<commit_message>
Add July ERAS Numbers
</commit_message>
<xml_diff>
--- a/docs/data/2024-07-29_eras_historic_data.xlsx
+++ b/docs/data/2024-07-29_eras_historic_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asnonline-my.sharepoint.com/personal/kpivert_asn-online_org/Documents/Desktop/dw/48_eras/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="36" documentId="8_{8395F4EE-5E2A-4DCB-BFAA-C5EB3D9FF82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{418144C9-DA5E-4A66-8066-DCE7189DAB91}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{8395F4EE-5E2A-4DCB-BFAA-C5EB3D9FF82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{879E7AA4-20DA-46F6-A963-60A56804606F}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229422FC-2505-4C8C-802C-C7E70C4F8B5F}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="00_Monthly" sheetId="1" r:id="rId1"/>
     <sheet name="01_Edu-Status" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,18 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="13">
-  <si>
-    <t>UK</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="13">
   <si>
     <t xml:space="preserve">ERAS </t>
   </si>
   <si>
     <t>month_year</t>
-  </si>
-  <si>
-    <t>edu_status</t>
   </si>
   <si>
     <t>num_candidate</t>
@@ -61,6 +58,12 @@
   </si>
   <si>
     <t>mean_apps_program</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>edu_status</t>
   </si>
   <si>
     <t>IMG</t>
@@ -82,7 +85,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,9 +164,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -201,7 +204,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -307,7 +310,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -449,7 +452,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -457,13 +460,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DD9739-02B2-44B0-87D8-0D3CE110A7C3}">
-  <dimension ref="A1:K69"/>
+  <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -475,30 +478,30 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11">
       <c r="A1" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="2">
         <v>2014</v>
       </c>
@@ -522,7 +525,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11">
       <c r="A3" s="2">
         <v>2014</v>
       </c>
@@ -545,7 +548,7 @@
         <v>19.472000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11">
       <c r="A4" s="2">
         <v>2014</v>
       </c>
@@ -568,7 +571,7 @@
         <v>3.3239999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11">
       <c r="A5" s="2">
         <v>2014</v>
       </c>
@@ -591,7 +594,7 @@
         <v>1.2050000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11">
       <c r="A6" s="2">
         <v>2014</v>
       </c>
@@ -614,7 +617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11">
       <c r="A7" s="2">
         <v>2014</v>
       </c>
@@ -637,7 +640,7 @@
         <v>2.7829999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11">
       <c r="A8" s="2">
         <v>2014</v>
       </c>
@@ -660,7 +663,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11">
       <c r="A9" s="2">
         <v>2014</v>
       </c>
@@ -683,7 +686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11">
       <c r="A10" s="2">
         <v>2014</v>
       </c>
@@ -706,7 +709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11">
       <c r="A11" s="2">
         <v>2014</v>
       </c>
@@ -729,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11">
       <c r="A12" s="2">
         <v>2015</v>
       </c>
@@ -752,7 +755,7 @@
         <v>58.804000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11">
       <c r="A13" s="2">
         <v>2015</v>
       </c>
@@ -775,7 +778,7 @@
         <v>10.676</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11">
       <c r="A14" s="2">
         <v>2015</v>
       </c>
@@ -798,7 +801,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11">
       <c r="A15" s="2">
         <v>2015</v>
       </c>
@@ -821,7 +824,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="2">
         <v>2015</v>
       </c>
@@ -844,7 +847,7 @@
         <v>1.304</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="2">
         <v>2015</v>
       </c>
@@ -867,7 +870,7 @@
         <v>2.5310000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="2">
         <v>2015</v>
       </c>
@@ -890,7 +893,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19" s="2">
         <v>2015</v>
       </c>
@@ -913,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20" s="2">
         <v>2015</v>
       </c>
@@ -936,7 +939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="2">
         <v>2015</v>
       </c>
@@ -959,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="2">
         <v>2016</v>
       </c>
@@ -982,7 +985,7 @@
         <v>44.273000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="2">
         <v>2016</v>
       </c>
@@ -1005,7 +1008,7 @@
         <v>9.7899999999999991</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="2">
         <v>2016</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>2.2370000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="2">
         <v>2016</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>1.671</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="2">
         <v>2016</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="2">
         <v>2016</v>
       </c>
@@ -1097,7 +1100,7 @@
         <v>2.6720000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7">
       <c r="A28" s="2">
         <v>2016</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7">
       <c r="A29" s="2">
         <v>2016</v>
       </c>
@@ -1143,7 +1146,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7">
       <c r="A30" s="2">
         <v>2016</v>
       </c>
@@ -1166,7 +1169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="2">
         <v>2016</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="2">
         <v>2016</v>
       </c>
@@ -1212,7 +1215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="2">
         <v>2017</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>37.119999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="2">
         <v>2017</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>6.68</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="2">
         <v>2017</v>
       </c>
@@ -1281,7 +1284,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="2">
         <v>2017</v>
       </c>
@@ -1304,7 +1307,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="2">
         <v>2017</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7">
       <c r="A38" s="2">
         <v>2017</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7">
       <c r="A39" s="2">
         <v>2018</v>
       </c>
@@ -1373,7 +1376,7 @@
         <v>38.700000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7">
       <c r="A40" s="2">
         <v>2018</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>7.13</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7">
       <c r="A41" s="2">
         <v>2018</v>
       </c>
@@ -1410,16 +1413,16 @@
         <v>347</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F41" s="2">
         <v>9.6300000000000008</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="2">
         <v>2018</v>
       </c>
@@ -1433,16 +1436,16 @@
         <v>107</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F42" s="2">
         <v>3.8</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="2">
         <v>2018</v>
       </c>
@@ -1456,16 +1459,16 @@
         <v>54</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F43" s="2">
         <v>4.5</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="2">
         <v>2019</v>
       </c>
@@ -1479,16 +1482,16 @@
         <v>5884</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F44" s="2">
         <v>20.79</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="2">
         <v>2019</v>
       </c>
@@ -1502,16 +1505,16 @@
         <v>1050</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F45" s="2">
         <v>14.8</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="2">
         <v>2019</v>
       </c>
@@ -1525,16 +1528,16 @@
         <v>486</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F46" s="2">
         <v>12.15</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="2">
         <v>2019</v>
       </c>
@@ -1548,16 +1551,16 @@
         <v>110</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F47" s="2">
         <v>5.79</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="2">
         <v>2020</v>
       </c>
@@ -1571,16 +1574,16 @@
         <v>5911</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F48" s="2">
         <v>21.97</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="2">
         <v>2020</v>
       </c>
@@ -1594,16 +1597,16 @@
         <v>883</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F49" s="2">
         <v>13.4</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="2">
         <v>2020</v>
       </c>
@@ -1617,16 +1620,16 @@
         <v>432</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F50" s="2">
         <v>10.3</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="2">
         <v>2020</v>
       </c>
@@ -1640,16 +1643,16 @@
         <v>298</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F51" s="2">
         <v>8.5</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="2">
         <v>2020</v>
       </c>
@@ -1663,16 +1666,16 @@
         <v>95</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F52" s="2">
         <v>7.9</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="2">
         <v>2021</v>
       </c>
@@ -1686,16 +1689,16 @@
         <v>9859</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F53" s="2">
         <v>25.7</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="2">
         <v>2021</v>
       </c>
@@ -1709,16 +1712,16 @@
         <v>872</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F54" s="7">
         <v>11.8</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="2">
         <v>2021</v>
       </c>
@@ -1732,16 +1735,16 @@
         <v>198</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F55" s="7">
         <v>6.8</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="2">
         <v>2021</v>
       </c>
@@ -1755,16 +1758,16 @@
         <v>67</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F56" s="7">
         <v>4.5</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="2">
         <v>2022</v>
       </c>
@@ -1778,16 +1781,16 @@
         <v>10402</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F57" s="7">
         <v>29.8</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="2">
         <v>2022</v>
       </c>
@@ -1801,16 +1804,16 @@
         <v>1232</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F58" s="7">
         <v>16.899999999999999</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="2">
         <v>2022</v>
       </c>
@@ -1824,16 +1827,16 @@
         <v>555</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F59" s="7">
         <v>11.3</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="2">
         <v>2022</v>
       </c>
@@ -1847,16 +1850,16 @@
         <v>149</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F60" s="7">
         <v>6.5</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="2">
         <v>2023</v>
       </c>
@@ -1870,16 +1873,16 @@
         <v>11112</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F61" s="7">
         <v>30.4</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="2">
         <v>2023</v>
       </c>
@@ -1893,16 +1896,16 @@
         <v>1196</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F62" s="7">
         <v>13</v>
       </c>
       <c r="G62" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="2">
         <v>2023</v>
       </c>
@@ -1916,16 +1919,16 @@
         <v>468</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F63" s="7">
         <v>9</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="2">
         <v>2023</v>
       </c>
@@ -1939,16 +1942,16 @@
         <v>175</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F64" s="7">
         <v>7.3</v>
       </c>
       <c r="G64" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="2">
         <v>2024</v>
       </c>
@@ -1962,16 +1965,16 @@
         <v>9569</v>
       </c>
       <c r="E65" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F65" s="7">
         <v>30.57</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="2">
         <v>2024</v>
       </c>
@@ -1985,16 +1988,16 @@
         <v>1282</v>
       </c>
       <c r="E66" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F66" s="7">
         <v>19.399999999999999</v>
       </c>
       <c r="G66" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="2">
         <v>2024</v>
       </c>
@@ -2008,16 +2011,16 @@
         <v>488</v>
       </c>
       <c r="E67" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F67" s="7">
         <v>13.6</v>
       </c>
       <c r="G67" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="2">
         <v>2024</v>
       </c>
@@ -2031,16 +2034,16 @@
         <v>198</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F68" s="7">
         <v>8.6</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="2">
         <v>2024</v>
       </c>
@@ -2054,13 +2057,36 @@
         <v>242</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F69" s="7">
         <v>4.32</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>0</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B70" s="3">
+        <v>45474</v>
+      </c>
+      <c r="C70" s="7">
+        <v>360</v>
+      </c>
+      <c r="D70" s="7">
+        <v>9998</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F70" s="7">
+        <v>27.8</v>
+      </c>
+      <c r="G70" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2071,13 +2097,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58110C59-B104-49D7-82F0-8B4AFB37B928}">
-  <dimension ref="A1:H109"/>
+  <dimension ref="A1:H112"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+    <sheetView topLeftCell="A83" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -2090,33 +2116,33 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="2">
         <v>2017</v>
       </c>
@@ -2142,7 +2168,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="2">
         <v>2017</v>
       </c>
@@ -2168,7 +2194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="2">
         <v>2017</v>
       </c>
@@ -2194,7 +2220,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
@@ -2220,7 +2246,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="2">
         <v>2017</v>
       </c>
@@ -2246,7 +2272,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="2">
         <v>2017</v>
       </c>
@@ -2272,7 +2298,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="2">
         <v>2017</v>
       </c>
@@ -2298,7 +2324,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="2">
         <v>2018</v>
       </c>
@@ -2324,7 +2350,7 @@
         <v>18.88</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="2">
         <v>2018</v>
       </c>
@@ -2350,7 +2376,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="2">
         <v>2018</v>
       </c>
@@ -2376,7 +2402,7 @@
         <v>4.28</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="2">
         <v>2018</v>
       </c>
@@ -2402,7 +2428,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="2">
         <v>2018</v>
       </c>
@@ -2428,7 +2454,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="2">
         <v>2018</v>
       </c>
@@ -2454,7 +2480,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="2">
         <v>2018</v>
       </c>
@@ -2480,7 +2506,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="2">
         <v>2018</v>
       </c>
@@ -2506,7 +2532,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="2">
         <v>2018</v>
       </c>
@@ -2532,7 +2558,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="2">
         <v>2018</v>
       </c>
@@ -2558,7 +2584,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="2">
         <v>2018</v>
       </c>
@@ -2584,7 +2610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="2">
         <v>2018</v>
       </c>
@@ -2610,7 +2636,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="2">
         <v>2018</v>
       </c>
@@ -2636,7 +2662,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="2">
         <v>2018</v>
       </c>
@@ -2662,7 +2688,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="2">
         <v>2018</v>
       </c>
@@ -2688,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="2">
         <v>2018</v>
       </c>
@@ -2714,7 +2740,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="2">
         <v>2018</v>
       </c>
@@ -2740,7 +2766,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="2">
         <v>2018</v>
       </c>
@@ -2766,7 +2792,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="2">
         <v>2018</v>
       </c>
@@ -2792,7 +2818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="2">
         <v>2018</v>
       </c>
@@ -2818,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="2">
         <v>2019</v>
       </c>
@@ -2844,7 +2870,7 @@
         <v>21.29</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30" s="2">
         <v>2019</v>
       </c>
@@ -2870,7 +2896,7 @@
         <v>8.36</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="2">
         <v>2019</v>
       </c>
@@ -2896,7 +2922,7 @@
         <v>5.27</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="2">
         <v>2019</v>
       </c>
@@ -2922,7 +2948,7 @@
         <v>9.16</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8">
       <c r="A33" s="2">
         <v>2019</v>
       </c>
@@ -2948,7 +2974,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8">
       <c r="A34" s="2">
         <v>2019</v>
       </c>
@@ -2974,7 +3000,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8">
       <c r="A35" s="2">
         <v>2019</v>
       </c>
@@ -3000,7 +3026,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8">
       <c r="A36" s="2">
         <v>2019</v>
       </c>
@@ -3026,7 +3052,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8">
       <c r="A37" s="2">
         <v>2019</v>
       </c>
@@ -3052,7 +3078,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8">
       <c r="A38" s="2">
         <v>2019</v>
       </c>
@@ -3078,7 +3104,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8">
       <c r="A39" s="2">
         <v>2019</v>
       </c>
@@ -3104,7 +3130,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8">
       <c r="A40" s="2">
         <v>2019</v>
       </c>
@@ -3130,7 +3156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:8">
       <c r="A41" s="2">
         <v>2019</v>
       </c>
@@ -3156,7 +3182,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:8">
       <c r="A42" s="2">
         <v>2019</v>
       </c>
@@ -3182,7 +3208,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8">
       <c r="A43" s="2">
         <v>2019</v>
       </c>
@@ -3208,7 +3234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8">
       <c r="A44" s="2">
         <v>2019</v>
       </c>
@@ -3234,7 +3260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8">
       <c r="A45" s="2">
         <v>2020</v>
       </c>
@@ -3260,7 +3286,7 @@
         <v>30.54</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8">
       <c r="A46" s="2">
         <v>2020</v>
       </c>
@@ -3286,7 +3312,7 @@
         <v>6.57</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8">
       <c r="A47" s="2">
         <v>2020</v>
       </c>
@@ -3312,7 +3338,7 @@
         <v>6.44</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8">
       <c r="A48" s="2">
         <v>2020</v>
       </c>
@@ -3338,7 +3364,7 @@
         <v>5.46</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8">
       <c r="A49" s="2">
         <v>2020</v>
       </c>
@@ -3364,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:8">
       <c r="A50" s="2">
         <v>2020</v>
       </c>
@@ -3390,7 +3416,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8">
       <c r="A51" s="2">
         <v>2020</v>
       </c>
@@ -3416,7 +3442,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8">
       <c r="A52" s="2">
         <v>2020</v>
       </c>
@@ -3442,7 +3468,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8">
       <c r="A53" s="2">
         <v>2020</v>
       </c>
@@ -3468,7 +3494,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8">
       <c r="A54" s="2">
         <v>2020</v>
       </c>
@@ -3494,7 +3520,7 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8">
       <c r="A55" s="2">
         <v>2020</v>
       </c>
@@ -3520,7 +3546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8">
       <c r="A56" s="2">
         <v>2020</v>
       </c>
@@ -3546,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8">
       <c r="A57" s="2">
         <v>2020</v>
       </c>
@@ -3572,7 +3598,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8">
       <c r="A58" s="2">
         <v>2020</v>
       </c>
@@ -3598,7 +3624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8">
       <c r="A59" s="2">
         <v>2021</v>
       </c>
@@ -3624,7 +3650,7 @@
         <v>51.65</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8">
       <c r="A60" s="2">
         <v>2021</v>
       </c>
@@ -3650,7 +3676,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8">
       <c r="A61" s="2">
         <v>2021</v>
       </c>
@@ -3676,7 +3702,7 @@
         <v>9.64</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8">
       <c r="A62" s="2">
         <v>2021</v>
       </c>
@@ -3702,7 +3728,7 @@
         <v>5.83</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8">
       <c r="A63" s="2">
         <v>2021</v>
       </c>
@@ -3728,7 +3754,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8">
       <c r="A64" s="2">
         <v>2021</v>
       </c>
@@ -3754,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8">
       <c r="A65" s="2">
         <v>2021</v>
       </c>
@@ -3780,7 +3806,7 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8">
       <c r="A66" s="2">
         <v>2021</v>
       </c>
@@ -3806,7 +3832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8">
       <c r="A67" s="2">
         <v>2021</v>
       </c>
@@ -3832,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8">
       <c r="A68" s="2">
         <v>2021</v>
       </c>
@@ -3858,7 +3884,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8">
       <c r="A69" s="2">
         <v>2021</v>
       </c>
@@ -3884,7 +3910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8">
       <c r="A70" s="2">
         <v>2021</v>
       </c>
@@ -3910,7 +3936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8">
       <c r="A71" s="2">
         <v>2022</v>
       </c>
@@ -3936,7 +3962,7 @@
         <v>47.38</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8">
       <c r="A72" s="2">
         <v>2022</v>
       </c>
@@ -3962,7 +3988,7 @@
         <v>12.64</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8">
       <c r="A73" s="2">
         <v>2022</v>
       </c>
@@ -3988,7 +4014,7 @@
         <v>10.96</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8">
       <c r="A74" s="2">
         <v>2022</v>
       </c>
@@ -4014,7 +4040,7 @@
         <v>6.52</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8">
       <c r="A75" s="2">
         <v>2022</v>
       </c>
@@ -4040,7 +4066,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8">
       <c r="A76" s="2">
         <v>2022</v>
       </c>
@@ -4066,7 +4092,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8">
       <c r="A77" s="2">
         <v>2022</v>
       </c>
@@ -4092,7 +4118,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8">
       <c r="A78" s="2">
         <v>2022</v>
       </c>
@@ -4118,7 +4144,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8">
       <c r="A79" s="2">
         <v>2022</v>
       </c>
@@ -4144,7 +4170,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8">
       <c r="A80" s="2">
         <v>2022</v>
       </c>
@@ -4170,7 +4196,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8">
       <c r="A81" s="2">
         <v>2022</v>
       </c>
@@ -4196,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8">
       <c r="A82" s="2">
         <v>2022</v>
       </c>
@@ -4222,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8">
       <c r="A83" s="2">
         <v>2023</v>
       </c>
@@ -4248,7 +4274,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8">
       <c r="A84" s="2">
         <v>2023</v>
       </c>
@@ -4274,7 +4300,7 @@
         <v>12.01</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8">
       <c r="A85" s="2">
         <v>2023</v>
       </c>
@@ -4300,7 +4326,7 @@
         <v>12.09</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8">
       <c r="A86" s="2">
         <v>2023</v>
       </c>
@@ -4326,7 +4352,7 @@
         <v>6.96</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8">
       <c r="A87" s="2">
         <v>2023</v>
       </c>
@@ -4352,7 +4378,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8">
       <c r="A88" s="2">
         <v>2023</v>
       </c>
@@ -4378,7 +4404,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8">
       <c r="A89" s="2">
         <v>2023</v>
       </c>
@@ -4404,7 +4430,7 @@
         <v>2.91</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8">
       <c r="A90" s="2">
         <v>2023</v>
       </c>
@@ -4430,7 +4456,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8">
       <c r="A91" s="2">
         <v>2023</v>
       </c>
@@ -4456,7 +4482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8">
       <c r="A92" s="2">
         <v>2023</v>
       </c>
@@ -4482,7 +4508,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8">
       <c r="A93" s="2">
         <v>2023</v>
       </c>
@@ -4508,7 +4534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8">
       <c r="A94" s="2">
         <v>2023</v>
       </c>
@@ -4534,7 +4560,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8">
       <c r="A95" s="2">
         <v>2024</v>
       </c>
@@ -4560,7 +4586,7 @@
         <v>43.77</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8">
       <c r="A96" s="2">
         <v>2024</v>
       </c>
@@ -4586,7 +4612,7 @@
         <v>12.02</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8">
       <c r="A97" s="2">
         <v>2024</v>
       </c>
@@ -4612,7 +4638,7 @@
         <v>9.43</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8">
       <c r="A98" s="2">
         <v>2024</v>
       </c>
@@ -4638,7 +4664,7 @@
         <v>7.24</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8">
       <c r="A99" s="2">
         <v>2024</v>
       </c>
@@ -4664,7 +4690,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8">
       <c r="A100" s="2">
         <v>2024</v>
       </c>
@@ -4690,7 +4716,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8">
       <c r="A101" s="2">
         <v>2024</v>
       </c>
@@ -4716,7 +4742,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8">
       <c r="A102" s="2">
         <v>2024</v>
       </c>
@@ -4742,7 +4768,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8">
       <c r="A103" s="2">
         <v>2024</v>
       </c>
@@ -4768,7 +4794,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8">
       <c r="A104" s="2">
         <v>2024</v>
       </c>
@@ -4794,7 +4820,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8">
       <c r="A105" s="2">
         <v>2024</v>
       </c>
@@ -4820,7 +4846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8">
       <c r="A106" s="2">
         <v>2024</v>
       </c>
@@ -4846,7 +4872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8">
       <c r="A107" s="2">
         <v>2024</v>
       </c>
@@ -4872,7 +4898,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8">
       <c r="A108" s="2">
         <v>2024</v>
       </c>
@@ -4898,7 +4924,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8">
       <c r="A109" s="2">
         <v>2024</v>
       </c>
@@ -4922,6 +4948,84 @@
       </c>
       <c r="H109" s="7">
         <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B110" s="3">
+        <v>45474</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" s="7">
+        <v>194</v>
+      </c>
+      <c r="E110" s="7">
+        <v>6857</v>
+      </c>
+      <c r="F110" s="7">
+        <v>148</v>
+      </c>
+      <c r="G110" s="7">
+        <v>35.35</v>
+      </c>
+      <c r="H110" s="7">
+        <v>46.33</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B111" s="3">
+        <v>45474</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" s="7">
+        <v>84</v>
+      </c>
+      <c r="E111" s="7">
+        <v>1895</v>
+      </c>
+      <c r="F111" s="7">
+        <v>148</v>
+      </c>
+      <c r="G111" s="7">
+        <v>22.56</v>
+      </c>
+      <c r="H111" s="7">
+        <v>12.98</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B112" s="3">
+        <v>45474</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D112" s="7">
+        <v>82</v>
+      </c>
+      <c r="E112" s="7">
+        <v>1246</v>
+      </c>
+      <c r="F112" s="7">
+        <v>148</v>
+      </c>
+      <c r="G112" s="7">
+        <v>15.2</v>
+      </c>
+      <c r="H112" s="7">
+        <v>8.9600000000000009</v>
       </c>
     </row>
   </sheetData>
@@ -4939,6 +5043,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C16F6BDF645AFA4DAA0562B4614D7463" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2190cffa455fc0c1e002531b4220c57">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0" xmlns:ns4="9d1ac0ca-1a98-4231-85a1-ed33c0acd435" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2053a201fa537a586296eb109384f981" ns3:_="" ns4:_="">
     <xsd:import namespace="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0"/>
@@ -5173,54 +5285,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60617E3-E230-476E-9CCF-0BA818870561}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60617E3-E230-476E-9CCF-0BA818870561}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25A2893D-E5A3-415A-BA36-9368EB896EBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0"/>
-    <ds:schemaRef ds:uri="9d1ac0ca-1a98-4231-85a1-ed33c0acd435"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1B25A75-AF8C-4D13-B2FA-4444A997F21D}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1B25A75-AF8C-4D13-B2FA-4444A997F21D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9d1ac0ca-1a98-4231-85a1-ed33c0acd435"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25A2893D-E5A3-415A-BA36-9368EB896EBC}"/>
 </file>
</xml_diff>

<commit_message>
Fix Text in Card
</commit_message>
<xml_diff>
--- a/docs/data/2024-07-29_eras_historic_data.xlsx
+++ b/docs/data/2024-07-29_eras_historic_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asnonline-my.sharepoint.com/personal/kpivert_asn-online_org/Documents/Desktop/dw/48_eras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asnonline-my.sharepoint.com/personal/kpivert_asn-online_org/Documents/Documents/01_gh/eras_2025/docs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{8395F4EE-5E2A-4DCB-BFAA-C5EB3D9FF82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{879E7AA4-20DA-46F6-A963-60A56804606F}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{8395F4EE-5E2A-4DCB-BFAA-C5EB3D9FF82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95C191BD-53ED-41E4-A12B-FACD1AF019D6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{229422FC-2505-4C8C-802C-C7E70C4F8B5F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{229422FC-2505-4C8C-802C-C7E70C4F8B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="00_Monthly" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="14">
   <si>
     <t xml:space="preserve">ERAS </t>
   </si>
@@ -77,6 +77,9 @@
   <si>
     <t>US DO</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -85,7 +88,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,10 +166,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -204,7 +211,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -310,7 +317,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -452,7 +459,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -462,11 +469,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DD9739-02B2-44B0-87D8-0D3CE110A7C3}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -478,7 +485,7 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -501,7 +508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2014</v>
       </c>
@@ -525,7 +532,7 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2014</v>
       </c>
@@ -548,7 +555,7 @@
         <v>19.472000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2014</v>
       </c>
@@ -571,7 +578,7 @@
         <v>3.3239999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2014</v>
       </c>
@@ -594,7 +601,7 @@
         <v>1.2050000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2014</v>
       </c>
@@ -617,7 +624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2014</v>
       </c>
@@ -640,7 +647,7 @@
         <v>2.7829999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2014</v>
       </c>
@@ -663,7 +670,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2014</v>
       </c>
@@ -686,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2014</v>
       </c>
@@ -709,7 +716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2014</v>
       </c>
@@ -732,7 +739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2015</v>
       </c>
@@ -755,7 +762,7 @@
         <v>58.804000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2015</v>
       </c>
@@ -778,7 +785,7 @@
         <v>10.676</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2015</v>
       </c>
@@ -801,7 +808,7 @@
         <v>4.88</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2015</v>
       </c>
@@ -824,7 +831,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2015</v>
       </c>
@@ -847,7 +854,7 @@
         <v>1.304</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2015</v>
       </c>
@@ -870,7 +877,7 @@
         <v>2.5310000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2015</v>
       </c>
@@ -893,7 +900,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2015</v>
       </c>
@@ -916,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>2015</v>
       </c>
@@ -939,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2015</v>
       </c>
@@ -962,7 +969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>2016</v>
       </c>
@@ -985,7 +992,7 @@
         <v>44.273000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>2016</v>
       </c>
@@ -1008,7 +1015,7 @@
         <v>9.7899999999999991</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>2016</v>
       </c>
@@ -1031,7 +1038,7 @@
         <v>2.2370000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>2016</v>
       </c>
@@ -1054,7 +1061,7 @@
         <v>1.671</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>2016</v>
       </c>
@@ -1077,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>2016</v>
       </c>
@@ -1100,7 +1107,7 @@
         <v>2.6720000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>2016</v>
       </c>
@@ -1123,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>2016</v>
       </c>
@@ -1146,7 +1153,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>2016</v>
       </c>
@@ -1169,7 +1176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>2016</v>
       </c>
@@ -1192,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>2016</v>
       </c>
@@ -1215,7 +1222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>2017</v>
       </c>
@@ -1238,7 +1245,7 @@
         <v>37.119999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>2017</v>
       </c>
@@ -1261,7 +1268,7 @@
         <v>6.68</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>2017</v>
       </c>
@@ -1284,7 +1291,7 @@
         <v>3.96</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>2017</v>
       </c>
@@ -1307,7 +1314,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>2017</v>
       </c>
@@ -1330,7 +1337,7 @@
         <v>1.22</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>2017</v>
       </c>
@@ -1353,7 +1360,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>2018</v>
       </c>
@@ -1376,7 +1383,7 @@
         <v>38.700000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>2018</v>
       </c>
@@ -1399,7 +1406,7 @@
         <v>7.13</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>2018</v>
       </c>
@@ -1422,7 +1429,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>2018</v>
       </c>
@@ -1445,7 +1452,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>2018</v>
       </c>
@@ -1468,7 +1475,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>2019</v>
       </c>
@@ -1491,7 +1498,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>2019</v>
       </c>
@@ -1514,7 +1521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>2019</v>
       </c>
@@ -1537,7 +1544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>2019</v>
       </c>
@@ -1560,7 +1567,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>2020</v>
       </c>
@@ -1583,7 +1590,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>2020</v>
       </c>
@@ -1606,7 +1613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>2020</v>
       </c>
@@ -1629,7 +1636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>2020</v>
       </c>
@@ -1652,7 +1659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>2020</v>
       </c>
@@ -1675,7 +1682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>2021</v>
       </c>
@@ -1698,7 +1705,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>2021</v>
       </c>
@@ -1721,7 +1728,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>2021</v>
       </c>
@@ -1744,7 +1751,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>2021</v>
       </c>
@@ -1767,7 +1774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>2022</v>
       </c>
@@ -1790,7 +1797,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>2022</v>
       </c>
@@ -1813,7 +1820,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>2022</v>
       </c>
@@ -1836,7 +1843,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>2022</v>
       </c>
@@ -1859,7 +1866,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>2023</v>
       </c>
@@ -1882,7 +1889,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>2023</v>
       </c>
@@ -1905,7 +1912,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>2023</v>
       </c>
@@ -1928,7 +1935,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>2023</v>
       </c>
@@ -1951,7 +1958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>2024</v>
       </c>
@@ -1974,7 +1981,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>2024</v>
       </c>
@@ -1997,7 +2004,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>2024</v>
       </c>
@@ -2020,7 +2027,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>2024</v>
       </c>
@@ -2043,7 +2050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>2024</v>
       </c>
@@ -2066,7 +2073,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>2025</v>
       </c>
@@ -2097,13 +2104,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58110C59-B104-49D7-82F0-8B4AFB37B928}">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G112" sqref="G112"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -2116,7 +2123,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2142,7 +2149,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2017</v>
       </c>
@@ -2168,7 +2175,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2017</v>
       </c>
@@ -2194,7 +2201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>2017</v>
       </c>
@@ -2220,7 +2227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2017</v>
       </c>
@@ -2246,7 +2253,7 @@
         <v>2.11</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>2017</v>
       </c>
@@ -2272,7 +2279,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>2017</v>
       </c>
@@ -2298,7 +2305,7 @@
         <v>1.1499999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>2017</v>
       </c>
@@ -2324,7 +2331,7 @@
         <v>1.56</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>2018</v>
       </c>
@@ -2350,7 +2357,7 @@
         <v>18.88</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>2018</v>
       </c>
@@ -2376,7 +2383,7 @@
         <v>7.05</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>2018</v>
       </c>
@@ -2402,7 +2409,7 @@
         <v>4.28</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>2018</v>
       </c>
@@ -2428,7 +2435,7 @@
         <v>9.52</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>2018</v>
       </c>
@@ -2454,7 +2461,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>2018</v>
       </c>
@@ -2480,7 +2487,7 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>2018</v>
       </c>
@@ -2506,7 +2513,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>2018</v>
       </c>
@@ -2532,7 +2539,7 @@
         <v>1.66</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>2018</v>
       </c>
@@ -2558,7 +2565,7 @@
         <v>1.94</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>2018</v>
       </c>
@@ -2584,7 +2591,7 @@
         <v>1.43</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>2018</v>
       </c>
@@ -2610,7 +2617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>2018</v>
       </c>
@@ -2636,7 +2643,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>2018</v>
       </c>
@@ -2662,7 +2669,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>2018</v>
       </c>
@@ -2688,7 +2695,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>2018</v>
       </c>
@@ -2714,7 +2721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>2018</v>
       </c>
@@ -2740,7 +2747,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>2018</v>
       </c>
@@ -2766,7 +2773,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>2018</v>
       </c>
@@ -2792,7 +2799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>2018</v>
       </c>
@@ -2818,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>2018</v>
       </c>
@@ -2844,7 +2851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>2019</v>
       </c>
@@ -2870,7 +2877,7 @@
         <v>21.29</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>2019</v>
       </c>
@@ -2896,7 +2903,7 @@
         <v>8.36</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>2019</v>
       </c>
@@ -2922,7 +2929,7 @@
         <v>5.27</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>2019</v>
       </c>
@@ -2948,7 +2955,7 @@
         <v>9.16</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>2019</v>
       </c>
@@ -2974,7 +2981,7 @@
         <v>3.88</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>2019</v>
       </c>
@@ -3000,7 +3007,7 @@
         <v>2.78</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>2019</v>
       </c>
@@ -3026,7 +3033,7 @@
         <v>1.49</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>2019</v>
       </c>
@@ -3052,7 +3059,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>2019</v>
       </c>
@@ -3078,7 +3085,7 @@
         <v>2.52</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>2019</v>
       </c>
@@ -3104,7 +3111,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>2019</v>
       </c>
@@ -3130,7 +3137,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>2019</v>
       </c>
@@ -3156,7 +3163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>2019</v>
       </c>
@@ -3182,7 +3189,7 @@
         <v>1.24</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>2019</v>
       </c>
@@ -3208,7 +3215,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>2019</v>
       </c>
@@ -3234,7 +3241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>2019</v>
       </c>
@@ -3260,7 +3267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>2020</v>
       </c>
@@ -3286,7 +3293,7 @@
         <v>30.54</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>2020</v>
       </c>
@@ -3312,7 +3319,7 @@
         <v>6.57</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>2020</v>
       </c>
@@ -3338,7 +3345,7 @@
         <v>6.44</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>2020</v>
       </c>
@@ -3364,7 +3371,7 @@
         <v>5.46</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>2020</v>
       </c>
@@ -3390,7 +3397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>2020</v>
       </c>
@@ -3416,7 +3423,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>2020</v>
       </c>
@@ -3442,7 +3449,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>2020</v>
       </c>
@@ -3468,7 +3475,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>2020</v>
       </c>
@@ -3494,7 +3501,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>2020</v>
       </c>
@@ -3520,7 +3527,7 @@
         <v>2.0499999999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>2020</v>
       </c>
@@ -3546,7 +3553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>2020</v>
       </c>
@@ -3572,7 +3579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>2020</v>
       </c>
@@ -3598,7 +3605,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>2020</v>
       </c>
@@ -3624,7 +3631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>2021</v>
       </c>
@@ -3650,7 +3657,7 @@
         <v>51.65</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>2021</v>
       </c>
@@ -3676,7 +3683,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>2021</v>
       </c>
@@ -3702,7 +3709,7 @@
         <v>9.64</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>2021</v>
       </c>
@@ -3728,7 +3735,7 @@
         <v>5.83</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>2021</v>
       </c>
@@ -3754,7 +3761,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>2021</v>
       </c>
@@ -3780,7 +3787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>2021</v>
       </c>
@@ -3806,7 +3813,7 @@
         <v>1.71</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>2021</v>
       </c>
@@ -3832,7 +3839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>2021</v>
       </c>
@@ -3858,7 +3865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>2021</v>
       </c>
@@ -3884,7 +3891,7 @@
         <v>1.33</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>2021</v>
       </c>
@@ -3910,7 +3917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>2021</v>
       </c>
@@ -3936,7 +3943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>2022</v>
       </c>
@@ -3962,7 +3969,7 @@
         <v>47.38</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>2022</v>
       </c>
@@ -3988,7 +3995,7 @@
         <v>12.64</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>2022</v>
       </c>
@@ -4014,7 +4021,7 @@
         <v>10.96</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>2022</v>
       </c>
@@ -4040,7 +4047,7 @@
         <v>6.52</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>2022</v>
       </c>
@@ -4066,7 +4073,7 @@
         <v>1.69</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>2022</v>
       </c>
@@ -4092,7 +4099,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>2022</v>
       </c>
@@ -4118,7 +4125,7 @@
         <v>3.41</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>2022</v>
       </c>
@@ -4144,7 +4151,7 @@
         <v>1.29</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>2022</v>
       </c>
@@ -4170,7 +4177,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>2022</v>
       </c>
@@ -4196,7 +4203,7 @@
         <v>1.36</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>2022</v>
       </c>
@@ -4222,7 +4229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>2022</v>
       </c>
@@ -4248,7 +4255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>2023</v>
       </c>
@@ -4274,7 +4281,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>2023</v>
       </c>
@@ -4300,7 +4307,7 @@
         <v>12.01</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>2023</v>
       </c>
@@ -4326,7 +4333,7 @@
         <v>12.09</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>2023</v>
       </c>
@@ -4352,7 +4359,7 @@
         <v>6.96</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>2023</v>
       </c>
@@ -4378,7 +4385,7 @@
         <v>1.48</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>2023</v>
       </c>
@@ -4404,7 +4411,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>2023</v>
       </c>
@@ -4430,7 +4437,7 @@
         <v>2.91</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>2023</v>
       </c>
@@ -4456,7 +4463,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>2023</v>
       </c>
@@ -4482,7 +4489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>2023</v>
       </c>
@@ -4508,7 +4515,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>2023</v>
       </c>
@@ -4534,7 +4541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>2023</v>
       </c>
@@ -4560,7 +4567,7 @@
         <v>1.1299999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>2024</v>
       </c>
@@ -4586,7 +4593,7 @@
         <v>43.77</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>2024</v>
       </c>
@@ -4612,7 +4619,7 @@
         <v>12.02</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>2024</v>
       </c>
@@ -4638,7 +4645,7 @@
         <v>9.43</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>2024</v>
       </c>
@@ -4664,7 +4671,7 @@
         <v>7.24</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>2024</v>
       </c>
@@ -4690,7 +4697,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>2024</v>
       </c>
@@ -4716,7 +4723,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>2024</v>
       </c>
@@ -4742,7 +4749,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>2024</v>
       </c>
@@ -4768,7 +4775,7 @@
         <v>1.21</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>2024</v>
       </c>
@@ -4794,7 +4801,7 @@
         <v>1.1599999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>2024</v>
       </c>
@@ -4820,7 +4827,7 @@
         <v>1.72</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>2024</v>
       </c>
@@ -4846,7 +4853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>2024</v>
       </c>
@@ -4872,7 +4879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>2024</v>
       </c>
@@ -4898,7 +4905,7 @@
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>2024</v>
       </c>
@@ -4924,7 +4931,7 @@
         <v>1.27</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="2">
         <v>2024</v>
       </c>
@@ -4950,7 +4957,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="2">
         <v>2025</v>
       </c>
@@ -4976,7 +4983,7 @@
         <v>46.33</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="2">
         <v>2025</v>
       </c>
@@ -5002,7 +5009,7 @@
         <v>12.98</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="2">
         <v>2025</v>
       </c>
@@ -5026,6 +5033,11 @@
       </c>
       <c r="H112" s="7">
         <v>8.9600000000000009</v>
+      </c>
+    </row>
+    <row r="118" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H118" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -5034,23 +5046,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C16F6BDF645AFA4DAA0562B4614D7463" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2190cffa455fc0c1e002531b4220c57">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0" xmlns:ns4="9d1ac0ca-1a98-4231-85a1-ed33c0acd435" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2053a201fa537a586296eb109384f981" ns3:_="" ns4:_="">
     <xsd:import namespace="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0"/>
@@ -5285,14 +5280,56 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60617E3-E230-476E-9CCF-0BA818870561}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25A2893D-E5A3-415A-BA36-9368EB896EBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0"/>
+    <ds:schemaRef ds:uri="9d1ac0ca-1a98-4231-85a1-ed33c0acd435"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1B25A75-AF8C-4D13-B2FA-4444A997F21D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1B25A75-AF8C-4D13-B2FA-4444A997F21D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25A2893D-E5A3-415A-BA36-9368EB896EBC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60617E3-E230-476E-9CCF-0BA818870561}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add August ERAS Data
</commit_message>
<xml_diff>
--- a/docs/data/2024-07-29_eras_historic_data.xlsx
+++ b/docs/data/2024-07-29_eras_historic_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://asnonline-my.sharepoint.com/personal/kpivert_asn-online_org/Documents/Documents/01_gh/eras_2025/docs/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{8395F4EE-5E2A-4DCB-BFAA-C5EB3D9FF82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95C191BD-53ED-41E4-A12B-FACD1AF019D6}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{8395F4EE-5E2A-4DCB-BFAA-C5EB3D9FF82B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE8A569E-B34A-4154-83A8-C0BA66B8F0DE}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{229422FC-2505-4C8C-802C-C7E70C4F8B5F}"/>
+    <workbookView xWindow="7425" yWindow="1980" windowWidth="21600" windowHeight="11385" xr2:uid="{229422FC-2505-4C8C-802C-C7E70C4F8B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="00_Monthly" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="14">
   <si>
     <t xml:space="preserve">ERAS </t>
   </si>
@@ -164,10 +164,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DD9739-02B2-44B0-87D8-0D3CE110A7C3}">
-  <dimension ref="A1:K70"/>
+  <dimension ref="A1:K71"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2096,6 +2092,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A71" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B71" s="3">
+        <v>45505</v>
+      </c>
+      <c r="C71" s="7">
+        <v>62</v>
+      </c>
+      <c r="D71" s="7">
+        <v>766</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F71" s="7">
+        <v>12.35</v>
+      </c>
+      <c r="G71" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2106,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58110C59-B104-49D7-82F0-8B4AFB37B928}">
   <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H118" sqref="H118"/>
+    <sheetView topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4665,7 +4684,7 @@
         <v>148</v>
       </c>
       <c r="G98" s="7">
-        <v>31</v>
+        <v>19.829999999999998</v>
       </c>
       <c r="H98" s="7">
         <v>7.24</v>
@@ -4717,7 +4736,7 @@
         <v>148</v>
       </c>
       <c r="G100" s="7">
-        <v>19.829999999999998</v>
+        <v>31</v>
       </c>
       <c r="H100" s="7">
         <v>1.26</v>
@@ -5035,7 +5054,85 @@
         <v>8.9600000000000009</v>
       </c>
     </row>
-    <row r="118" spans="8:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B113" s="3">
+        <v>45505</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D113" s="7">
+        <v>50</v>
+      </c>
+      <c r="E113" s="7">
+        <v>613</v>
+      </c>
+      <c r="F113" s="7">
+        <v>148</v>
+      </c>
+      <c r="G113" s="7">
+        <v>12.26</v>
+      </c>
+      <c r="H113" s="7">
+        <v>4.17</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B114" s="3">
+        <v>45505</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D114" s="7">
+        <v>6</v>
+      </c>
+      <c r="E114" s="7">
+        <v>20</v>
+      </c>
+      <c r="F114" s="7">
+        <v>148</v>
+      </c>
+      <c r="G114" s="7">
+        <v>3.33</v>
+      </c>
+      <c r="H114" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B115" s="3">
+        <v>45505</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D115" s="7">
+        <v>6</v>
+      </c>
+      <c r="E115" s="7">
+        <v>133</v>
+      </c>
+      <c r="F115" s="7">
+        <v>148</v>
+      </c>
+      <c r="G115" s="7">
+        <v>22.17</v>
+      </c>
+      <c r="H115" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H118" s="1" t="s">
         <v>13</v>
       </c>
@@ -5046,6 +5143,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C16F6BDF645AFA4DAA0562B4614D7463" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2190cffa455fc0c1e002531b4220c57">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0" xmlns:ns4="9d1ac0ca-1a98-4231-85a1-ed33c0acd435" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2053a201fa537a586296eb109384f981" ns3:_="" ns4:_="">
     <xsd:import namespace="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0"/>
@@ -5280,24 +5394,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60617E3-E230-476E-9CCF-0BA818870561}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1B25A75-AF8C-4D13-B2FA-4444A997F21D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25A2893D-E5A3-415A-BA36-9368EB896EBC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5314,22 +5429,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1B25A75-AF8C-4D13-B2FA-4444A997F21D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d3ec8ca6-9845-4ca5-85d2-d40bb63eefa0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D60617E3-E230-476E-9CCF-0BA818870561}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>